<commit_message>
plot social media usage
</commit_message>
<xml_diff>
--- a/Dataset/Internet_Social_Media_facts/social_media_fact_sheet.xlsx
+++ b/Dataset/Internet_Social_Media_facts/social_media_fact_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jt18/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jt18/Google Drive/UNCC CLT DA Boot Camp - JT/Project-1-group-4/uncc-group4-project1/Dataset/internet_social_media_facts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DA960F2-AA7B-9A49-9B9A-67FAFD587B37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426DE9E7-D7A4-C84D-AB7B-17E70B0A6BA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="2200" windowWidth="16860" windowHeight="16800" firstSheet="3" activeTab="11" xr2:uid="{65E6FD14-D1EB-F54D-BAD6-7846D4D6EA5F}"/>
+    <workbookView xWindow="11540" yWindow="680" windowWidth="14640" windowHeight="18500" activeTab="1" xr2:uid="{65E6FD14-D1EB-F54D-BAD6-7846D4D6EA5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1306,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0967C584-201A-EE47-AD86-4E29A947B9F1}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1410,14 +1410,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFA6DD0-89E5-E743-8916-0A898A9EF815}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>